<commit_message>
NAND and NOR 2 and 3 inputs
</commit_message>
<xml_diff>
--- a/Seminario de solución de circuitos digitales/NAND3/NAND3/Inversor.xlsx
+++ b/Seminario de solución de circuitos digitales/NAND3/NAND3/Inversor.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daniel\UDG\7mo\Seminario de solución de circuitos digitales\Inversor\Inversor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daniel\UDG\7mo\Seminario de solución de circuitos digitales\NAND3\NAND3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74714CA3-5566-4A15-8FB0-4DB465C4EA6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC401189-6A25-4B8B-BBBA-00E45C1E3D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NMOS" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,6 @@
     <sheet name="4mA" sheetId="5" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1779,8 +1778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAA9D475-0FA9-4E9E-AAAC-74C84BEAD93E}">
   <dimension ref="C1:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1824,7 +1823,7 @@
       </c>
       <c r="N2" s="7">
         <f>+I8*3</f>
-        <v>141</v>
+        <v>399</v>
       </c>
     </row>
     <row r="3" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1845,7 +1844,7 @@
       </c>
       <c r="N3" s="2">
         <f>+N2/2</f>
-        <v>70.5</v>
+        <v>199.5</v>
       </c>
     </row>
     <row r="4" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1916,7 +1915,7 @@
         <v>12</v>
       </c>
       <c r="I7" s="2">
-        <v>14.1</v>
+        <v>37.799999999999997</v>
       </c>
     </row>
     <row r="8" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1931,8 +1930,7 @@
         <v>21</v>
       </c>
       <c r="I8" s="2">
-        <f>+I7/0.3</f>
-        <v>47</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1971,7 +1969,7 @@
       </c>
       <c r="J12" s="7">
         <f>+I8+4</f>
-        <v>51</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.3">
@@ -1995,7 +1993,7 @@
       </c>
       <c r="J13" s="15">
         <f>+I8</f>
-        <v>47</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2019,7 +2017,7 @@
       </c>
       <c r="J14" s="11">
         <f>+I8+4</f>
-        <v>51</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2031,8 +2029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3E93690-D089-44DF-A0FA-47B8B48ADE81}">
   <dimension ref="C1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2077,7 +2075,7 @@
       </c>
       <c r="N2" s="7">
         <f>+I8*3</f>
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2098,7 +2096,7 @@
       </c>
       <c r="N3" s="2">
         <f>+N2/2</f>
-        <v>133.5</v>
+        <v>130.5</v>
       </c>
     </row>
     <row r="4" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2184,8 +2182,7 @@
         <v>21</v>
       </c>
       <c r="I8" s="2">
-        <f>+I7/0.3</f>
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -2224,7 +2221,7 @@
       </c>
       <c r="J12" s="7">
         <f>+I8+4</f>
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.3">
@@ -2248,7 +2245,7 @@
       </c>
       <c r="J13" s="15">
         <f>+I8</f>
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2272,7 +2269,7 @@
       </c>
       <c r="J14" s="11">
         <f>+I8+4</f>
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2285,7 +2282,7 @@
   <dimension ref="C1:N14"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2330,7 +2327,7 @@
       </c>
       <c r="N2" s="7">
         <f>+I8*3</f>
-        <v>396</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2351,7 +2348,7 @@
       </c>
       <c r="N3" s="2">
         <f>+N2/2</f>
-        <v>198</v>
+        <v>67.5</v>
       </c>
     </row>
     <row r="4" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2422,7 +2419,8 @@
         <v>12</v>
       </c>
       <c r="I7" s="2">
-        <v>39.6</v>
+        <f>+I8*0.3</f>
+        <v>13.5</v>
       </c>
     </row>
     <row r="8" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2437,8 +2435,7 @@
         <v>21</v>
       </c>
       <c r="I8" s="2">
-        <f>+I7/0.3</f>
-        <v>132</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -2477,7 +2474,7 @@
       </c>
       <c r="J12" s="7">
         <f>+I8+4</f>
-        <v>136</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.3">
@@ -2501,7 +2498,7 @@
       </c>
       <c r="J13" s="15">
         <f>+I8</f>
-        <v>132</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2525,7 +2522,7 @@
       </c>
       <c r="J14" s="11">
         <f>+I8+4</f>
-        <v>136</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>